<commit_message>
graph no plotting exch
</commit_message>
<xml_diff>
--- a/CIVICS_Ghana/Calliope_Ghana/Ghana-10Nodes/Graph_inputs.xlsx
+++ b/CIVICS_Ghana/Calliope_Ghana/Ghana-10Nodes/Graph_inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://feemit-my.sharepoint.com/personal/federica_inzoli_feem_it/Documents/REP/CIVICS Ghana/Ghana Energy Model/African Energy/Ghana-10Nodes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stevo\Repositories\CIVICS\CIVICS_Ghana\Calliope_Ghana\Ghana-10Nodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="114_{F2ECB4F9-0A1C-45C9-A0A1-E2506AFEE5E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{918559F3-4C56-4395-9AF3-20A7FF235C9B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A0517A-B806-4467-AC59-E1E61B31C341}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="6" xr2:uid="{9FB00E9D-CEB3-42BA-85F0-61134DCC4F6B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="3" xr2:uid="{9FB00E9D-CEB3-42BA-85F0-61134DCC4F6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Consumption Techs" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="105">
   <si>
     <t>Tech</t>
   </si>
@@ -130,21 +130,6 @@
   </si>
   <si>
     <t>Western Region</t>
-  </si>
-  <si>
-    <t>Hydro_Old</t>
-  </si>
-  <si>
-    <t>Hydro_New</t>
-  </si>
-  <si>
-    <t>CCGT</t>
-  </si>
-  <si>
-    <t>GT</t>
-  </si>
-  <si>
-    <t>ICE</t>
   </si>
   <si>
     <t>PV</t>
@@ -812,7 +797,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -823,7 +808,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -834,7 +819,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -845,7 +830,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -856,7 +841,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -867,7 +852,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -878,7 +863,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -889,7 +874,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -900,7 +885,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -911,7 +896,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -927,7 +912,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -952,7 +937,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -963,7 +948,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -974,7 +959,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -985,7 +970,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -996,7 +981,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1007,7 +992,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1023,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF150A4-DE49-47F1-B3B1-E0F51365CAAD}">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H19" sqref="G19:H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1043,29 +1028,29 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -1076,39 +1061,39 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="J7" s="3"/>
       <c r="N7" s="6"/>
@@ -1116,283 +1101,283 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
         <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
         <v>16</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
         <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
         <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
         <v>20</v>
@@ -1403,46 +1388,46 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
         <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B35" t="s">
         <v>18</v>
       </c>
       <c r="C35" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
         <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B37" t="s">
         <v>20</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -1500,10 +1485,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1511,10 +1496,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1522,10 +1507,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1533,10 +1518,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1544,10 +1529,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1555,10 +1540,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1566,10 +1551,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1577,10 +1562,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1588,10 +1573,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1599,10 +1584,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1630,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1638,7 +1623,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1650,7 +1635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A79EFBBC-D91E-4893-86C8-C299F0E0C218}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1669,7 +1654,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1677,7 +1662,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alpha parameter in graph function
</commit_message>
<xml_diff>
--- a/CIVICS_Ghana/Calliope_Ghana/Ghana-10Nodes/Graph_inputs.xlsx
+++ b/CIVICS_Ghana/Calliope_Ghana/Ghana-10Nodes/Graph_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stevo\Repositories\CIVICS\CIVICS_Ghana\Calliope_Ghana\Ghana-10Nodes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\payam\Documents\GitHub\CIVICS_Kenya\CIVICS_Ghana\Calliope_Ghana\Ghana-10Nodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACD3D91-3D69-454C-BAD4-D964B9055521}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F902BE02-3F63-4FFF-B125-D9FA9C011636}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-210" windowWidth="21840" windowHeight="13290" activeTab="6" xr2:uid="{9FB00E9D-CEB3-42BA-85F0-61134DCC4F6B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{9FB00E9D-CEB3-42BA-85F0-61134DCC4F6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Consumption Techs" sheetId="1" r:id="rId1"/>
@@ -468,7 +468,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -484,7 +484,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -786,12 +786,12 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -800,7 +800,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -825,12 +825,12 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
@@ -838,7 +838,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -849,7 +849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -860,7 +860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -871,7 +871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -882,7 +882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -893,7 +893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -904,7 +904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -915,7 +915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -926,7 +926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -937,7 +937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -961,13 +961,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -978,7 +978,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -989,7 +989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1058,13 +1058,13 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1118,7 +1118,7 @@
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -1131,7 +1131,7 @@
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1145,7 +1145,7 @@
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1157,7 +1157,7 @@
       </c>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>17</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>18</v>
       </c>
@@ -1512,13 +1512,13 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1649,14 +1649,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1682,20 +1682,20 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>